<commit_message>
update upstream sectors (coal, NG, crude oil) for EMH project
</commit_message>
<xml_diff>
--- a/csv/policies/reference/Ref_OBPS/formula_Ref_OBPS_BC.xlsx
+++ b/csv/policies/reference/Ref_OBPS/formula_Ref_OBPS_BC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\xCIMS\cims-models\csv\policies\reference\Ref_OBPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EB8FDED-F7CA-4C55-AC6D-85241AA0C507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7087E2E-A3D1-4ED7-A6F5-461E40140BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40545" yWindow="3660" windowWidth="17280" windowHeight="8880" xr2:uid="{E39D89C5-5E89-466A-9F02-8C675C99ACAC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E39D89C5-5E89-466A-9F02-8C675C99ACAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,12 +107,6 @@
     <t>$/tCO2e</t>
   </si>
   <si>
-    <t>CIMS.CAN.BC.Natural Gas Extraction</t>
-  </si>
-  <si>
-    <t>Natural Gas Extraction</t>
-  </si>
-  <si>
     <t>CIMS.CAN.BC.Petroleum Crude</t>
   </si>
   <si>
@@ -159,6 +153,12 @@
   </si>
   <si>
     <t>Transportation Equipment</t>
+  </si>
+  <si>
+    <t>Natural Gas Production</t>
+  </si>
+  <si>
+    <t>CIMS.CAN.BC.Natural Gas Production</t>
   </si>
 </sst>
 </file>
@@ -224,11 +224,23 @@
       <sheetName val="Demand"/>
       <sheetName val="Conversions"/>
       <sheetName val="Coefficients"/>
+      <sheetName val="Macro inputs"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0">
+        <row r="38">
+          <cell r="B38" t="str">
+            <v>Residential</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2">
+        <row r="2">
+          <cell r="K2">
+            <v>2000</v>
+          </cell>
+        </row>
         <row r="26">
           <cell r="K26">
             <v>0</v>
@@ -268,7 +280,14 @@
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="6">
+        <row r="1">
+          <cell r="G1">
+            <v>2000</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -594,17 +613,17 @@
   <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:X12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -678,7 +697,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -751,9 +770,9 @@
         <v>4.5789061745779298</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -762,7 +781,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
         <v>17</v>
@@ -824,9 +843,9 @@
         <v>4.5789061745779298</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -835,7 +854,7 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>
@@ -897,9 +916,9 @@
         <v>4.5789061745779298</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -908,7 +927,7 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
         <v>17</v>
@@ -970,9 +989,9 @@
         <v>4.5789061745779298</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -981,7 +1000,7 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
         <v>17</v>
@@ -1043,9 +1062,9 @@
         <v>4.5789061745779298</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -1054,7 +1073,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
         <v>17</v>
@@ -1116,9 +1135,9 @@
         <v>4.5789061745779298</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -1127,7 +1146,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G9" t="s">
         <v>17</v>
@@ -1189,9 +1208,9 @@
         <v>4.5789061745779298</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -1200,7 +1219,7 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G10" t="s">
         <v>17</v>
@@ -1262,9 +1281,9 @@
         <v>4.5789061745779298</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -1273,7 +1292,7 @@
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
         <v>17</v>
@@ -1335,9 +1354,9 @@
         <v>4.5789061745779298</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -1346,7 +1365,7 @@
         <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G12" t="s">
         <v>17</v>

</xml_diff>